<commit_message>
update style for excel 2017.12.21
</commit_message>
<xml_diff>
--- a/learnEXCEL/example_write.xlsx
+++ b/learnEXCEL/example_write.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="First Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Happy2017" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Middle Sheet two" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="First Sheet Copy" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -378,4 +380,40 @@
   <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>